<commit_message>
Stag Url s Added to excel sheet
</commit_message>
<xml_diff>
--- a/src/main/java/Excel_Lib/sysco_com_urls.xlsx
+++ b/src/main/java/Excel_Lib/sysco_com_urls.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin Lambert\Documents\Works\QE_Image\SyscoComWebsiteAutomation\src\main\java\Excel_Lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin Lambert\Documents\Works\QE_Image\SyscoComSiteAutomation\src\main\java\Excel_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4BBEEA-36F8-4863-9CBE-93B40F5D7738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7071B229-0053-424E-BD24-6356AC56AFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{176A4602-1A9B-4AE5-93DC-7E24DCEBABA8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{176A4602-1A9B-4AE5-93DC-7E24DCEBABA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="682">
   <si>
     <t>URL</t>
   </si>
@@ -1486,6 +1487,603 @@
   </si>
   <si>
     <t>http://titans-sysco-com-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/DDG/Cincinnati-become-a-customer.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL </t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Portico.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Data-Breach-Notification.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Newport-Meat.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Portland.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Market-Corner.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Los-Angeles.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Seafood/Buckhead-New-Jersey.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Specialty.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Intermountain.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/delivery.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Indianapolis.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Bakers-Source.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Company-Profile/Our-Purpose.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Safety-Data-Sheets.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/BuckheadMidAtlantic/BuckheadMidAtlantic-New-Customers.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Metro-New-York.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Acadiana.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Solutions-and-Services/Culinary-and-Product-Solutions.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/demo.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Western-Minnesota.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Kevin-Hourican-in-the-Media.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Ventura.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Sysco-Today.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Kansas-City.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Our-People/Diversity-and-Inclusion.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Jade-Mountain.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customers/Who-We-Serve/Higher-Education.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Riverside.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-Minnesota.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Jackson.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Raleigh.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Montana.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/San-Francisco.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Company-Profile/The-Sysco-Story.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Nashville.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Philadelphia.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Suppliers.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Sacramento.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Quality-Assurance/Specialty-Produce.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Seafood.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Houston.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Suppliers/Supplier-Partnerships.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Palisades-Ranch.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Baraboo.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Long-Island.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Knoxville.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customers/Who-We-Serve.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-Central-Florida.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/specialty.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Our-People/Our-Management.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Las-Vegas.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/BuckheadMidAtlantic.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Newport-Portland.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/BuckheadMidAtlantic/BuckheadMidAtlantic-History.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Solutions-and-Services/Technology-Solutions.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Oklahoma.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Block-and-Barrel.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Citavo.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/North-Texas.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-Denver.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Solutions-and-Services/Specialty-Companies.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Spokane.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Eastern-Wisconsin.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/San-Diego.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Elevating-the-Customer-Experience---Centralized-Customer-Care.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-Houston.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Solutions-and-Services/Services.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Our-People/FromSyscoCEO.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customers/Who-We-Serve/Restaurants.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/BuckheadMidAtlantic/BuckheadMidAtlantic-Careers.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Thought-Leadership.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Wholesome-Farms.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Newport-Palisades.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customers/Who-We-Serve/Healthcare-and-Senior-Living.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/St-Louis.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Eastern-Maryland.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Seafood/IncredibleFish/Sustainability-Initiatives.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/BuckheadMidAtlantic/BuckheadMidAtlantic-News-Room.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Albany.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Hawaii.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Pittsburgh.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Memphis.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customers/Who-We-Serve/Leisure.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Grand-Rapids.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Jacksonville.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/New-Orleans.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Connecticut.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/EarthPlus.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Newport-Pride.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Central-California.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/West-Coast-Florida.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/PerksTerms.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Company-Profile/Annual-Report.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Solutions-and-Services/Multicultural-Resources.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Alaska.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Arizona.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Charlotte.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Seafood/Trinity-Seafood.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Hampton-Roads.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/System-Usage-Policy.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customers.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customer-Letters.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Butchers-Block.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Seafood/Buckhead-South-Florida.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Asian-Foods.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-North-Carolina.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-Chicago.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Arkansas.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/House-Recipe.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Central-Illinois.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customers/Who-We-Serve/Food-Service-Management.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Suppliers/Supplier-Partnerships/Supplier-Resources.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Seafood/North-Star-Seafood.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Company-Profile/Public-Policy-Engagement.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-Boston.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Sysco-Today/Events.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Crown1-Enterprises.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Lincoln.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Newport-Northern-California.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/international-food-group.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Product-Categories.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-Ohio.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/BuckheadMidAtlantic/BuckheadMidAtlantic-Chef-Resources.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Arrezzio.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Our-People.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Seafood/Buckhead-Orlando.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/North-Dakota.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Newport-Meat/Newport-Products.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Cleveland.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Buckhead-Pride.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Atlanta.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Seafood/IncredibleFish.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Minnesota.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/terms.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Idaho.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/csr2020report.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Central-Florida.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-Atlanta.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Southeast-Florida.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Sysco-FreshPoint-Natural.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/New-Mexico.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Syracuse.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-San-Antonio.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customers/Who-We-Serve/Travel.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Company-Profile.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/traysys.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Central-Texas.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About/Sysco-Today/News-Room.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Quality-Assurance.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Contact-Us.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Foodie.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/East-Texas.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Central-Alabama.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Columbia.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-Dallas.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Cincinnati.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Casa-Solana.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Northern-New-England.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Louisville.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Solutions-and-Services.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/West-Texas.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Privacy-Notice.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Sysco-Global-Data-Processing-Addendum.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Chicago.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Detroit.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Gulf-Coast.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customers/Who-We-Serve/Government.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Baltimore.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Seattle.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Central-Pennsylvania.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/shopmobile.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Virginia.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Specialty-Meat-and-Seafood/Specialty-Meat/Buckhead-New-York.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/South-Florida.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Products/Sysco-Brand-Family/Fire-River-Farms.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Denver.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Boston.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Customers/Who-We-Serve/Retail.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Products/Solutions-and-Services/Culinary-and-Product-Solutions/Supplies-on-the-Fly.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Suppliers/Supplier-Partnerships/Supplier-Diversity.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/About.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Sysco-Applicant-Privacy-Notice.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Contact/Contact/Our-Locations/Iowa.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/Emergency-Response.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/portal/outage/logout.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/portal/outage/offlineurl.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/portal/outage/sessiontimedout.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/portal/outage/missingcredential.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/portal/outage/continuesession.html</t>
+  </si>
+  <si>
+    <t>https://sysco-com-staging-fastly.cxws-websites.sysco-go.com/portal/outage/invalidlogin.html</t>
   </si>
 </sst>
 </file>
@@ -1517,7 +2115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1528,6 +2126,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1559,7 +2163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1571,6 +2175,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3380,8 +3987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5C73AE-923C-4973-9DB7-9C4DC72F45FD}">
   <dimension ref="A1:A242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="G227" sqref="G227"/>
+    <sheetView topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="F230" sqref="F230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4602,4 +5209,1018 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AEFF3B7-D069-420A-8F6C-78B73A720979}">
+  <dimension ref="A1:A199"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="162.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>681</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>